<commit_message>
-menambahkan authorization dengan 4 role user yang memiliki akses berbeda -perbaikan bug pagination -perbaikan bug navbar -menambahkan fitur change password, dan create user
</commit_message>
<xml_diff>
--- a/public/AsetData/datadummyAset.xlsx
+++ b/public/AsetData/datadummyAset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DD7841-0F25-4F06-9F4E-83E91A33FA0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162DFF4B-6F10-4C2E-BB15-A2637329D3CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,31 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
-  <si>
-    <t>nama_aset</t>
-  </si>
-  <si>
-    <t>merek</t>
-  </si>
-  <si>
-    <t>kondisi</t>
-  </si>
-  <si>
-    <t>lokasi</t>
-  </si>
-  <si>
-    <t>jumlah_satuan</t>
-  </si>
-  <si>
-    <t>tanggal_pembelian</t>
-  </si>
-  <si>
-    <t>harga_pembelian</t>
-  </si>
-  <si>
-    <t>keterangan</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Laptop</t>
   </si>
@@ -110,15 +86,24 @@
   </si>
   <si>
     <t>Digunakan untuk menyimpan data perusahaan</t>
+  </si>
+  <si>
+    <t>2024-02-02</t>
+  </si>
+  <si>
+    <t>2024-03-21</t>
+  </si>
+  <si>
+    <t>2024-03-22</t>
+  </si>
+  <si>
+    <t>2024-03-23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -182,14 +167,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,10 +392,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -439,151 +423,125 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="1">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2">
+        <v>7500000</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="2">
-        <v>45292</v>
-      </c>
-      <c r="G2" s="3">
-        <v>7500000</v>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1200000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2">
+        <v>500000</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>45122</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1200000</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2">
-        <v>45359</v>
-      </c>
-      <c r="G4" s="3">
-        <v>500000</v>
+        <v>5</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1000000</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1">
-        <v>5</v>
-      </c>
-      <c r="F5" s="2">
-        <v>44915</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1000000</v>
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="2">
+        <v>5000000</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45436</v>
-      </c>
-      <c r="G6" s="3">
-        <v>5000000</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
+    <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>